<commit_message>
we are ading the project excel reader mail sender
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/data.xlsx
+++ b/src/test/resources/excel/data.xlsx
@@ -3,20 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ercan\Documents\workspaces\eclipse-ide-for-java-developers\Teplate1\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C076983-1112-435E-9347-1138AB821AC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{950C961D-8F4B-4308-A711-7C3BA7FE6C2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="29130" windowHeight="16500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginpagewebelement" sheetId="1" r:id="rId1"/>
     <sheet name="CurtainTrackOnly" sheetId="2" r:id="rId2"/>
+    <sheet name="loginAsWorker" sheetId="3" r:id="rId3"/>
+    <sheet name="Test_suite" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:V31"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>webElement</t>
   </si>
@@ -89,13 +87,46 @@
   </si>
   <si>
     <t>ProjectName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>ercan@ontherighttrack.com</t>
+  </si>
+  <si>
+    <t>Amerika254</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>loginAsWorker</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>CurtainTrackOnly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +148,20 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -135,15 +180,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,34 +481,52 @@
     <col min="1" max="1" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -471,10 +537,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D6FCA7-4372-4D15-87F2-77AE8821C7ED}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +548,7 @@
     <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -513,8 +579,11 @@
       <c r="J1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -544,6 +613,109 @@
       </c>
       <c r="J2">
         <v>7</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3677BA4D-4579-4966-85A9-76996D405720}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1A7B5CD4-9A46-478C-99D5-D3EF65F0C9E1}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAA0907E-5FB5-4C79-84FF-72F9ECABA7E8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>